<commit_message>
sesion persistente 1 día
</commit_message>
<xml_diff>
--- a/paginas/lista_cadetes/Lista_cadetes.xlsx
+++ b/paginas/lista_cadetes/Lista_cadetes.xlsx
@@ -85048,7 +85048,9 @@
       <c r="AC711" t="s">
         <v>7235</v>
       </c>
-      <c r="AD711"/>
+      <c r="AD711" t="s">
+        <v>7220</v>
+      </c>
       <c r="AE711"/>
       <c r="AF711"/>
       <c r="AG711"/>

</xml_diff>